<commit_message>
added sex split for supplement
</commit_message>
<xml_diff>
--- a/figures/Table Figure 2.xlsx
+++ b/figures/Table Figure 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/urai/Documents/code/int-brain-lab/citricAcid/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{633CA7C0-85CA-0849-886A-EBC1A178D1A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFE119D-3240-A64C-A65A-A6020359A176}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="0" windowWidth="31780" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,19 +382,27 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
       <bottom style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </bottom>
@@ -404,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -446,35 +454,47 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -28755,7 +28775,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
+  <pageSetup pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
 
@@ -28764,94 +28784,94 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:8" s="16" customFormat="1" ht="51">
       <c r="A1" s="8"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="14">
       <c r="A5" s="4"/>
@@ -28868,5 +28888,6 @@
     <mergeCell ref="B4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>